<commit_message>
Monthly inpatient cost updated
</commit_message>
<xml_diff>
--- a/data-raw/costs_inpt.xlsx
+++ b/data-raw/costs_inpt.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11110"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB76D41A-B056-5648-AC7D-1A9D02DECC9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="9640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_inpt" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>state_name</t>
   </si>
@@ -40,9 +46,6 @@
   </si>
   <si>
     <t>ref</t>
-  </si>
-  <si>
-    <t>None. Currently assuming same as P1/S2</t>
   </si>
   <si>
     <t>skinner2018healthcare</t>
@@ -51,7 +54,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -84,18 +91,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -107,7 +108,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -116,18 +117,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
+    <cellStyle name="Comma" xfId="8" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -135,10 +143,18 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -463,19 +479,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="100.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -489,48 +505,53 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <f>B3</f>
         <v>7699</v>
       </c>
-      <c r="C2" s="1">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="5">
+        <f>B2*((12358-6551)/3.92)/9454</f>
+        <v>1206.3809779253356</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>7699</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
+      <c r="B3" s="1">
+        <v>12577</v>
+      </c>
+      <c r="C3" s="5">
+        <f>B3*((12358-6551)/3.92)/9454</f>
+        <v>1970.730427245999</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>12577</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="5">
+        <f>B4*((12358-6551)/3.92)/9454</f>
+        <v>1970.730427245999</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated raw inpatient and outpatient cost
</commit_message>
<xml_diff>
--- a/data-raw/costs_inpt.xlsx
+++ b/data-raw/costs_inpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB76D41A-B056-5648-AC7D-1A9D02DECC9B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6AC9AF-490A-3241-AACD-3DA41F546BFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="9640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="580" yWindow="9440" windowWidth="11380" windowHeight="5820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_inpt" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,8 +513,8 @@
         <v>7699</v>
       </c>
       <c r="C2" s="5">
-        <f>B2*((12358-6551)/3.92)/9454</f>
-        <v>1206.3809779253356</v>
+        <f>ROUND(B2*((12358-6551)/3.92)/9454,0)</f>
+        <v>1206</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>7</v>
@@ -528,8 +528,8 @@
         <v>12577</v>
       </c>
       <c r="C3" s="5">
-        <f>B3*((12358-6551)/3.92)/9454</f>
-        <v>1970.730427245999</v>
+        <f>ROUND(B3*((12358-6551)/3.92)/9454,0)</f>
+        <v>1971</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>7</v>
@@ -543,8 +543,8 @@
         <v>12577</v>
       </c>
       <c r="C4" s="5">
-        <f>B4*((12358-6551)/3.92)/9454</f>
-        <v>1970.730427245999</v>
+        <f>ROUND(B4*((12358-6551)/3.92)/9454,0)</f>
+        <v>1971</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
inpatient and outpatient costs S1, set max duration IO therapy 2L+ to 2 years
</commit_message>
<xml_diff>
--- a/data-raw/costs_inpt.xlsx
+++ b/data-raw/costs_inpt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeroenjansen/Egnyte/Shared/RW GENERAL (MANAGEMENT)/Jeroen only access/IVI/GitHub/IVI-NSCLC/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A6FCA0-ECB6-4F44-99F3-95D35A5098D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE93694-5161-0E49-8B69-C0C1A5A2CBB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="4820" windowWidth="11380" windowHeight="5820" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21820" yWindow="11200" windowWidth="12860" windowHeight="8900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_inpt" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>state_name</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>skinner2018healthcare</t>
+  </si>
+  <si>
+    <t>Graham2018BIA</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -505,17 +508,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>0</v>
+        <f>ROUND(1.2*(1375.84+121.61+93.2),0)</f>
+        <v>1909</v>
       </c>
       <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4"/>
+        <f>ROUND(B2*((2927.15-1027.33)/3.92)/1971.79,0)</f>
+        <v>469</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">

</xml_diff>